<commit_message>
Shorten the data dictionary valid values sheet suffix.
To "-vl", allowing for Excel editing of the exported data dictionary for case types with names up to 28 chars in length. (Excel has a 31 character limit on sheet names).

Refs QA-3457
</commit_message>
<xml_diff>
--- a/corehq/apps/data_dictionary/tests/data/broken_data_dictionary.xlsx
+++ b/corehq/apps/data_dictionary/tests/data/broken_data_dictionary.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="caseType1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="caseType1-valid-values" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="caseType1-vl" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="caseType2" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -163,8 +163,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -191,57 +195,57 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -268,67 +272,67 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -354,57 +358,57 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Update data dictionary export/import...
To export the "display" value for the data types, and accept the same.

This makes editing of the data dictionary via web UI have the same names for data types as the export/import.
</commit_message>
<xml_diff>
--- a/corehq/apps/data_dictionary/tests/data/broken_data_dictionary.xlsx
+++ b/corehq/apps/data_dictionary/tests/data/broken_data_dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="caseType1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t xml:space="preserve">Case Property</t>
   </si>
@@ -42,19 +42,25 @@
     <t xml:space="preserve">dateprop</t>
   </si>
   <si>
-    <t xml:space="preserve">date</t>
+    <t xml:space="preserve">Date</t>
   </si>
   <si>
     <t xml:space="preserve">plainprop</t>
   </si>
   <si>
-    <t xml:space="preserve">plain</t>
+    <t xml:space="preserve">Plain</t>
   </si>
   <si>
     <t xml:space="preserve">selectprop</t>
   </si>
   <si>
-    <t xml:space="preserve">select</t>
+    <t xml:space="preserve">Multiple Choice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nonsense</t>
   </si>
   <si>
     <t xml:space="preserve">Valid Value</t>
@@ -189,13 +195,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -247,6 +253,17 @@
       </c>
       <c r="E4" s="1" t="n">
         <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -268,21 +285,21 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -290,10 +307,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -301,31 +318,31 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -333,7 +350,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -355,10 +372,10 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
updates bulk upload to support new field
</commit_message>
<xml_diff>
--- a/corehq/apps/data_dictionary/tests/data/broken_data_dictionary.xlsx
+++ b/corehq/apps/data_dictionary/tests/data/broken_data_dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="caseType1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,9 +22,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t xml:space="preserve">Case Property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Required</t>
   </si>
   <si>
     <t xml:space="preserve">Group</t>
@@ -195,15 +198,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.56640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -219,51 +222,58 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="B4" s="1"/>
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="F4" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="B5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -286,71 +296,71 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.56640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -369,15 +379,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.56640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -393,39 +403,45 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="B4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
change import and export for label
</commit_message>
<xml_diff>
--- a/corehq/apps/data_dictionary/tests/data/broken_data_dictionary.xlsx
+++ b/corehq/apps/data_dictionary/tests/data/broken_data_dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="caseType1" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,6 +27,9 @@
     <t xml:space="preserve">Case Property</t>
   </si>
   <si>
+    <t xml:space="preserve">Label</t>
+  </si>
+  <si>
     <t xml:space="preserve">Group</t>
   </si>
   <si>
@@ -36,19 +39,16 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Label</t>
-  </si>
-  <si>
     <t xml:space="preserve">Deprecated</t>
   </si>
   <si>
     <t xml:space="preserve">dateprop</t>
   </si>
   <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
     <t xml:space="preserve">Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
   </si>
   <si>
     <t xml:space="preserve">plainprop</t>
@@ -175,8 +175,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -203,82 +207,82 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="F:F E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="F2" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="F4" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="F5" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -301,70 +305,70 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="F:F B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -386,67 +390,70 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F:F"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.69"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="F2" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="F4" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
extend unit test for broken import
</commit_message>
<xml_diff>
--- a/corehq/apps/data_dictionary/tests/data/broken_data_dictionary.xlsx
+++ b/corehq/apps/data_dictionary/tests/data/broken_data_dictionary.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t xml:space="preserve">Case Property</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t xml:space="preserve">Nonsense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32foobar</t>
   </si>
   <si>
     <t xml:space="preserve">Valid Value</t>
@@ -201,18 +204,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.72"/>
   </cols>
   <sheetData>
@@ -283,6 +287,17 @@
         <v>14</v>
       </c>
       <c r="F5" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -298,7 +313,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -308,17 +323,17 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -326,10 +341,10 @@
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -337,31 +352,31 @@
         <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -369,7 +384,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -384,7 +399,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -394,7 +409,7 @@
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.69"/>
   </cols>

</xml_diff>